<commit_message>
TD3 and SAC unbounded action space
</commit_message>
<xml_diff>
--- a/th_rl/scenarios.xlsx
+++ b/th_rl/scenarios.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="9">
   <si>
     <t xml:space="preserve">agent</t>
   </si>
@@ -43,22 +43,10 @@
     <t xml:space="preserve">nactions</t>
   </si>
   <si>
-    <t xml:space="preserve">Reinforce</t>
-  </si>
-  <si>
     <t xml:space="preserve">ActorCritic</t>
   </si>
   <si>
-    <t xml:space="preserve">DQN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PPO</t>
-  </si>
-  <si>
     <t xml:space="preserve">SAC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DDPG</t>
   </si>
 </sst>
 </file>
@@ -157,7 +145,7 @@
   <dimension ref="A1:G41"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E49" activeCellId="0" sqref="E49"/>
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -193,10 +181,10 @@
         <v>1</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="D2" s="0" t="n">
-        <v>50000</v>
+        <v>1000</v>
       </c>
       <c r="E2" s="0" t="n">
         <v>0</v>
@@ -213,13 +201,13 @@
         <v>7</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="D3" s="0" t="n">
-        <v>50000</v>
+        <v>1000</v>
       </c>
       <c r="E3" s="0" t="n">
         <v>0</v>
@@ -236,13 +224,13 @@
         <v>7</v>
       </c>
       <c r="B4" s="0" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C4" s="0" t="n">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="D4" s="0" t="n">
-        <v>50000</v>
+        <v>1000</v>
       </c>
       <c r="E4" s="0" t="n">
         <v>0</v>
@@ -259,13 +247,13 @@
         <v>7</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="D5" s="0" t="n">
-        <v>50000</v>
+        <v>1000</v>
       </c>
       <c r="E5" s="0" t="n">
         <v>0</v>
@@ -285,19 +273,19 @@
         <v>1</v>
       </c>
       <c r="C6" s="0" t="n">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="D6" s="0" t="n">
-        <v>50000</v>
+        <v>1000</v>
       </c>
       <c r="E6" s="0" t="n">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="F6" s="0" t="n">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="G6" s="0" t="n">
-        <v>20</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -308,19 +296,19 @@
         <v>2</v>
       </c>
       <c r="C7" s="0" t="n">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="D7" s="0" t="n">
-        <v>50000</v>
+        <v>1000</v>
       </c>
       <c r="E7" s="0" t="n">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="F7" s="0" t="n">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="G7" s="0" t="n">
-        <v>20</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -328,22 +316,22 @@
         <v>7</v>
       </c>
       <c r="B8" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C8" s="0" t="n">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="D8" s="0" t="n">
-        <v>50000</v>
+        <v>1000</v>
       </c>
       <c r="E8" s="0" t="n">
-        <v>0.13</v>
+        <v>0</v>
       </c>
       <c r="F8" s="0" t="n">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="G8" s="0" t="n">
-        <v>20</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -351,36 +339,36 @@
         <v>7</v>
       </c>
       <c r="B9" s="0" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C9" s="0" t="n">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="D9" s="0" t="n">
-        <v>50000</v>
+        <v>1000</v>
       </c>
       <c r="E9" s="0" t="n">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="F9" s="0" t="n">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="G9" s="0" t="n">
-        <v>20</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B10" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C10" s="0" t="n">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="D10" s="0" t="n">
-        <v>50000</v>
+        <v>1000</v>
       </c>
       <c r="E10" s="0" t="n">
         <v>0</v>
@@ -394,16 +382,16 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>2</v>
       </c>
       <c r="C11" s="0" t="n">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="D11" s="0" t="n">
-        <v>50000</v>
+        <v>1000</v>
       </c>
       <c r="E11" s="0" t="n">
         <v>0</v>
@@ -417,16 +405,16 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>3</v>
       </c>
       <c r="C12" s="0" t="n">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="D12" s="0" t="n">
-        <v>50000</v>
+        <v>1000</v>
       </c>
       <c r="E12" s="0" t="n">
         <v>0</v>
@@ -440,16 +428,16 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B13" s="0" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C13" s="0" t="n">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="D13" s="0" t="n">
-        <v>50000</v>
+        <v>1000</v>
       </c>
       <c r="E13" s="0" t="n">
         <v>0</v>
@@ -463,108 +451,108 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B14" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C14" s="0" t="n">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="D14" s="0" t="n">
-        <v>50000</v>
+        <v>1000</v>
       </c>
       <c r="E14" s="0" t="n">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="F14" s="0" t="n">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="G14" s="0" t="n">
-        <v>20</v>
+        <v>100</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B15" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C15" s="0" t="n">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="D15" s="0" t="n">
-        <v>50000</v>
+        <v>1000</v>
       </c>
       <c r="E15" s="0" t="n">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="F15" s="0" t="n">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="G15" s="0" t="n">
-        <v>20</v>
+        <v>100</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>3</v>
       </c>
       <c r="C16" s="0" t="n">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="D16" s="0" t="n">
-        <v>50000</v>
+        <v>1000</v>
       </c>
       <c r="E16" s="0" t="n">
-        <v>0.13</v>
+        <v>0</v>
       </c>
       <c r="F16" s="0" t="n">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="G16" s="0" t="n">
-        <v>20</v>
+        <v>100</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C17" s="0" t="n">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="D17" s="0" t="n">
-        <v>50000</v>
+        <v>1000</v>
       </c>
       <c r="E17" s="0" t="n">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="F17" s="0" t="n">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="G17" s="0" t="n">
-        <v>20</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B18" s="0" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C18" s="0" t="n">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="D18" s="0" t="n">
-        <v>50000</v>
+        <v>1000</v>
       </c>
       <c r="E18" s="0" t="n">
         <v>0</v>
@@ -578,16 +566,16 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B19" s="0" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C19" s="0" t="n">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="D19" s="0" t="n">
-        <v>50000</v>
+        <v>1000</v>
       </c>
       <c r="E19" s="0" t="n">
         <v>0</v>
@@ -601,16 +589,16 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B20" s="0" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C20" s="0" t="n">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="D20" s="0" t="n">
-        <v>50000</v>
+        <v>1000</v>
       </c>
       <c r="E20" s="0" t="n">
         <v>0</v>
@@ -624,16 +612,16 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C21" s="0" t="n">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="D21" s="0" t="n">
-        <v>50000</v>
+        <v>1000</v>
       </c>
       <c r="E21" s="0" t="n">
         <v>0</v>
@@ -647,108 +635,108 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C22" s="0" t="n">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="D22" s="0" t="n">
-        <v>50000</v>
+        <v>1000</v>
       </c>
       <c r="E22" s="0" t="n">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="F22" s="0" t="n">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="G22" s="0" t="n">
-        <v>20</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B23" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C23" s="0" t="n">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="D23" s="0" t="n">
-        <v>50000</v>
+        <v>1000</v>
       </c>
       <c r="E23" s="0" t="n">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="F23" s="0" t="n">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="G23" s="0" t="n">
-        <v>20</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B24" s="0" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C24" s="0" t="n">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="D24" s="0" t="n">
-        <v>50000</v>
+        <v>1000</v>
       </c>
       <c r="E24" s="0" t="n">
-        <v>0.13</v>
+        <v>0</v>
       </c>
       <c r="F24" s="0" t="n">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="G24" s="0" t="n">
-        <v>20</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B25" s="0" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C25" s="0" t="n">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="D25" s="0" t="n">
-        <v>50000</v>
+        <v>1000</v>
       </c>
       <c r="E25" s="0" t="n">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="F25" s="0" t="n">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="G25" s="0" t="n">
-        <v>20</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C26" s="0" t="n">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="D26" s="0" t="n">
-        <v>50000</v>
+        <v>1000</v>
       </c>
       <c r="E26" s="0" t="n">
         <v>0</v>
@@ -757,21 +745,21 @@
         <v>1</v>
       </c>
       <c r="G26" s="0" t="n">
-        <v>100</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B27" s="0" t="n">
         <v>2</v>
       </c>
       <c r="C27" s="0" t="n">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="D27" s="0" t="n">
-        <v>50000</v>
+        <v>1000</v>
       </c>
       <c r="E27" s="0" t="n">
         <v>0</v>
@@ -780,21 +768,21 @@
         <v>1</v>
       </c>
       <c r="G27" s="0" t="n">
-        <v>100</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B28" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C28" s="0" t="n">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="D28" s="0" t="n">
-        <v>50000</v>
+        <v>1000</v>
       </c>
       <c r="E28" s="0" t="n">
         <v>0</v>
@@ -803,21 +791,21 @@
         <v>1</v>
       </c>
       <c r="G28" s="0" t="n">
-        <v>100</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B29" s="0" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C29" s="0" t="n">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="D29" s="0" t="n">
-        <v>50000</v>
+        <v>1000</v>
       </c>
       <c r="E29" s="0" t="n">
         <v>0</v>
@@ -826,113 +814,113 @@
         <v>1</v>
       </c>
       <c r="G29" s="0" t="n">
-        <v>100</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B30" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C30" s="0" t="n">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="D30" s="0" t="n">
-        <v>50000</v>
+        <v>1000</v>
       </c>
       <c r="E30" s="0" t="n">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="F30" s="0" t="n">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="G30" s="0" t="n">
-        <v>20</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B31" s="0" t="n">
         <v>2</v>
       </c>
       <c r="C31" s="0" t="n">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="D31" s="0" t="n">
-        <v>50000</v>
+        <v>1000</v>
       </c>
       <c r="E31" s="0" t="n">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="F31" s="0" t="n">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="G31" s="0" t="n">
-        <v>20</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B32" s="0" t="n">
         <v>3</v>
       </c>
       <c r="C32" s="0" t="n">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="D32" s="0" t="n">
-        <v>50000</v>
+        <v>1000</v>
       </c>
       <c r="E32" s="0" t="n">
-        <v>0.13</v>
+        <v>0</v>
       </c>
       <c r="F32" s="0" t="n">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="G32" s="0" t="n">
-        <v>20</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B33" s="0" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C33" s="0" t="n">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="D33" s="0" t="n">
-        <v>50000</v>
+        <v>1000</v>
       </c>
       <c r="E33" s="0" t="n">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="F33" s="0" t="n">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="G33" s="0" t="n">
-        <v>20</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B34" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C34" s="0" t="n">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="D34" s="0" t="n">
-        <v>50000</v>
+        <v>1000</v>
       </c>
       <c r="E34" s="0" t="n">
         <v>0</v>
@@ -946,16 +934,16 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B35" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C35" s="0" t="n">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="D35" s="0" t="n">
-        <v>50000</v>
+        <v>1000</v>
       </c>
       <c r="E35" s="0" t="n">
         <v>0</v>
@@ -969,16 +957,16 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B36" s="0" t="n">
         <v>3</v>
       </c>
       <c r="C36" s="0" t="n">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="D36" s="0" t="n">
-        <v>50000</v>
+        <v>1000</v>
       </c>
       <c r="E36" s="0" t="n">
         <v>0</v>
@@ -992,16 +980,16 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B37" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C37" s="0" t="n">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="D37" s="0" t="n">
-        <v>50000</v>
+        <v>1000</v>
       </c>
       <c r="E37" s="0" t="n">
         <v>0</v>
@@ -1015,16 +1003,16 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B38" s="0" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C38" s="0" t="n">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="D38" s="0" t="n">
-        <v>50000</v>
+        <v>1000</v>
       </c>
       <c r="E38" s="0" t="n">
         <v>0</v>
@@ -1038,16 +1026,16 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B39" s="0" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C39" s="0" t="n">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="D39" s="0" t="n">
-        <v>50000</v>
+        <v>1000</v>
       </c>
       <c r="E39" s="0" t="n">
         <v>0</v>
@@ -1061,16 +1049,16 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B40" s="0" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C40" s="0" t="n">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="D40" s="0" t="n">
-        <v>50000</v>
+        <v>1000</v>
       </c>
       <c r="E40" s="0" t="n">
         <v>0</v>
@@ -1084,16 +1072,16 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B41" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C41" s="0" t="n">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="D41" s="0" t="n">
-        <v>50000</v>
+        <v>1000</v>
       </c>
       <c r="E41" s="0" t="n">
         <v>0</v>

</xml_diff>